<commit_message>
Unicode to string TAF conversion
Now able to read TAF as string
</commit_message>
<xml_diff>
--- a/testbed.xlsx
+++ b/testbed.xlsx
@@ -1,57 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17870"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob\Documents\Python Scripts\MEF Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4090"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
-    <t>Newark Liberty International Airport</t>
+    <t>Minneapolis-St Paul Internationa</t>
   </si>
   <si>
-    <t xml:space="preserve">KEWR 132325Z 1400/1506 13007KT P6SM FEW140 BKN250 
-            FM140300 07008KT P6SM OVC060 
-            TEMPO 1403/1405 2SM -SN OVC025 
-            FM140500 05014G23KT 3/4SM -SN OVC008 
-            FM140800 03022G33KT 1/4SM SN BLSN FZFG VV002 
-            FM141000 03028G39KT 1/4SM +SN BLSN FZFG VV002 
-            FM142000 33025G34KT 2SM -SN OVC015 
-            FM150200 30020G30KT 4SM -SN OVC035 
-            FM150400 29017G28KT P6SM BKN040
+    <t xml:space="preserve">KMSP 152048Z 1521/1624 20007KT P6SM FEW250 
+            FM160100 16005KT P6SM FEW200 
+            FM161200 14010KT P6SM BKN050 OVC100
           </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -67,27 +57,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -387,27 +368,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="56.54296875" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" width="56.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row customHeight="1" ht="72.5" r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="145" x14ac:dyDescent="0.35">
+    <row customHeight="1" ht="145" r="2" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added time-end to hazards
Used a while loop to solve [i+1] index error problem.

Need to address tempo group time structure difference
</commit_message>
<xml_diff>
--- a/testbed.xlsx
+++ b/testbed.xlsx
@@ -16,13 +16,17 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
-    <t>Minneapolis-St Paul Internationa</t>
+    <t>Wright-Patterson Air Force Base</t>
   </si>
   <si>
-    <t xml:space="preserve">KMSP 162335Z 1700/1806 14017G24KT P6SM OVC090 
-            FM170800 16005KT P6SM OVC018 
-            FM171400 26008KT P6SM SCT020 
-            FM171700 28016G28KT P6SM BKN035
+    <t xml:space="preserve">TAF KFFO 201900Z 2019/2201 18012KT 9000 -SHRA SCT040 QNH2995INS 
+            TEMPO 2020/2024 31015G25KT -TSRAGS BKN020CB OVC030 
+            BECMG 2100/2101 33009KT 9000 -RA FEW020 OVC035 QNH2993INS 
+            BECMG 2102/2103 12006KT 4800 -RA BR SCT005 BKN020 OVC035 QNH2991INS 
+            BECMG 2104/2105 10006KT 3200 -DZ BR SCT005 OVC009 QNH2992INS 
+            BECMG 2105/2106 22006KT 3200 -DZ BR OVC005 QNH2993INS 
+            BECMG 2112/2113 33009KT 4800 BR SCT005 BKN010 QNH3006INS 
+            BECMG 2115/2116 35009KT 9999 NSW FEW020 BKN120 QNH3008INS TX13/2021Z TN07/2115Z
           </t>
   </si>
 </sst>

</xml_diff>